<commit_message>
redo part2 after redoing day11
</commit_message>
<xml_diff>
--- a/22/d22_p1(in_exc).xlsx
+++ b/22/d22_p1(in_exc).xlsx
@@ -15,7 +15,7 @@
     <sheet name="in_exc" sheetId="1" r:id="rId1"/>
     <sheet name="Data Sort" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -3045,7 +3045,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3064,6 +3064,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3077,12 +3083,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -20193,8 +20200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M990"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A944" workbookViewId="0">
-      <selection activeCell="N952" sqref="N952"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20287,7 +20294,7 @@
       <c r="I3">
         <v>0</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="5">
         <v>92</v>
       </c>
       <c r="K3">

</xml_diff>